<commit_message>
ALL exchange logic added to income statement
</commit_message>
<xml_diff>
--- a/docs/Issue Tracker.xlsx
+++ b/docs/Issue Tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kenrm\repositories\fin-trade-extract\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{984220AB-CB41-409B-A7BF-B6288475DD2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C51E925A-07D5-4014-9A69-1E7AB51D8B88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{C4FC26E6-3159-49DB-8833-BD64C3B31EA8}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="27">
   <si>
     <t>WORKFLOW</t>
   </si>
@@ -56,9 +56,6 @@
     <t>PROBLEM</t>
   </si>
   <si>
-    <t>PULLS ALL QUARTERS</t>
-  </si>
-  <si>
     <t>PRIVATE KEY WORKS</t>
   </si>
   <si>
@@ -87,6 +84,39 @@
   </si>
   <si>
     <t>etf profile</t>
+  </si>
+  <si>
+    <t>UPDATE RUN TIME</t>
+  </si>
+  <si>
+    <t>UPDATE DAY</t>
+  </si>
+  <si>
+    <t>DAILY</t>
+  </si>
+  <si>
+    <t>FRIDAY</t>
+  </si>
+  <si>
+    <t>UPDATE TIME</t>
+  </si>
+  <si>
+    <t>NO SCHEDULE</t>
+  </si>
+  <si>
+    <t>BULK WATERMARK</t>
+  </si>
+  <si>
+    <t>EXCHANGE FILTER ALL</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>not printing iters to log</t>
+  </si>
+  <si>
+    <t>UPDATE CREDIT CONSUMPTION</t>
   </si>
 </sst>
 </file>
@@ -122,8 +152,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="18" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -458,10 +489,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{039E647E-7EBC-453E-8A2B-FDCBCA09C5DE}">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:K10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -470,9 +501,13 @@
     <col min="2" max="2" width="9.6328125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18.6328125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="17.54296875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.1796875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.54296875" customWidth="1"/>
+    <col min="7" max="7" width="22.6328125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -483,27 +518,60 @@
         <v>5</v>
       </c>
       <c r="D1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G1" t="s">
         <v>7</v>
       </c>
-      <c r="E1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="H1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J1" t="s">
+        <v>20</v>
+      </c>
+      <c r="K1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="D2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2" t="s">
+        <v>2</v>
+      </c>
+      <c r="G2" t="s">
+        <v>2</v>
+      </c>
+      <c r="H2">
+        <v>40</v>
+      </c>
+      <c r="I2" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2" s="1">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -513,40 +581,136 @@
       <c r="D3" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E4" t="s">
+        <v>2</v>
+      </c>
+      <c r="F4" t="s">
+        <v>2</v>
+      </c>
+      <c r="G4" t="s">
+        <v>2</v>
+      </c>
+      <c r="H4">
+        <v>65</v>
+      </c>
+      <c r="K4">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
+      <c r="B6" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" t="s">
+        <v>25</v>
+      </c>
+      <c r="D6" t="s">
+        <v>4</v>
+      </c>
+      <c r="F6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" t="s">
+        <v>2</v>
+      </c>
+      <c r="I7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" t="s">
+        <v>2</v>
+      </c>
+      <c r="D9" t="s">
+        <v>2</v>
+      </c>
+      <c r="E9" t="s">
+        <v>24</v>
+      </c>
+      <c r="F9" t="s">
+        <v>24</v>
+      </c>
+      <c r="G9" t="s">
+        <v>24</v>
+      </c>
+      <c r="H9">
+        <v>10</v>
+      </c>
+      <c r="I9" t="s">
+        <v>18</v>
+      </c>
+      <c r="J9" s="1">
+        <v>1.0416666666666666E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
-        <v>15</v>
+      <c r="B10" t="s">
+        <v>2</v>
+      </c>
+      <c r="D10" t="s">
+        <v>2</v>
+      </c>
+      <c r="E10" t="s">
+        <v>24</v>
+      </c>
+      <c r="F10" t="s">
+        <v>24</v>
+      </c>
+      <c r="G10" t="s">
+        <v>24</v>
+      </c>
+      <c r="H10">
+        <v>10</v>
+      </c>
+      <c r="I10" t="s">
+        <v>18</v>
+      </c>
+      <c r="J10" s="1">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>